<commit_message>
Real Estate Powerpoint Push 12-12
</commit_message>
<xml_diff>
--- a/outputs/Financial_Model.xlsx
+++ b/outputs/Financial_Model.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1428" uniqueCount="257">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1458" uniqueCount="254">
   <si>
     <t>Revenue and COGS Build</t>
   </si>
@@ -55,49 +55,49 @@
     <t>Frequency Source</t>
   </si>
   <si>
-    <t>Scaffolding Rental Services</t>
+    <t>Custom Vehicle Up-fitting</t>
   </si>
   <si>
-    <t>Average project rental cost</t>
+    <t>Standard rate for full vehicle modification</t>
   </si>
   <si>
-    <t>Consistent demand for scaffolding services across various projects</t>
+    <t>Monthly volume as projected from backlog estimates</t>
   </si>
   <si>
-    <t>Custom Scaffold Design</t>
+    <t>Gold Division Prepackaged Systems</t>
   </si>
   <si>
-    <t>Design services priced based on complexity</t>
+    <t>Price for standardized power systems package</t>
   </si>
   <si>
-    <t>Custom jobs with multiple components</t>
+    <t>Regular orders, indicative of stable client base</t>
   </si>
   <si>
-    <t>Sales of Construction Materials</t>
+    <t>Generator Sales</t>
   </si>
   <si>
-    <t>Materials consistently in demand</t>
+    <t>Retail sales of Honda generators and pumps</t>
   </si>
   <si>
-    <t>Regular sales for ongoing constructions</t>
+    <t>Estimated based on past year performance</t>
   </si>
   <si>
-    <t>Safety Training Programs</t>
+    <t>Consulting and Advisory Services</t>
   </si>
   <si>
-    <t>Added value service for clients</t>
+    <t>Support services for OEM clients</t>
   </si>
   <si>
-    <t>Training sessions scheduled throughout the month</t>
+    <t>Consulting engagements expected monthly</t>
   </si>
   <si>
-    <t>Equipment Leasing</t>
+    <t>Miscellaneous Parts and Accessories</t>
   </si>
   <si>
-    <t>Short-term leasing for client projects</t>
+    <t>Add-on parts and upgrades</t>
   </si>
   <si>
-    <t>Steady interest from varied industrial sectors</t>
+    <t>High volume due to broad accessory range</t>
   </si>
   <si>
     <t>Total</t>
@@ -118,49 +118,49 @@
     <t>Cost Source</t>
   </si>
   <si>
-    <t>Material Costs</t>
+    <t>Steel for Vehicle Construction</t>
   </si>
   <si>
-    <t>Incurred consistently across projects</t>
+    <t>Used in most vehicle customizations</t>
   </si>
   <si>
-    <t>Materials are replenished monthly</t>
+    <t>Projected based on high demand periods</t>
   </si>
   <si>
-    <t>Outsourced Labor</t>
+    <t>Electrical Components</t>
   </si>
   <si>
-    <t>Specialty subcontractors for specific projects</t>
+    <t>Components for customizing vehicle electrical systems</t>
   </si>
   <si>
-    <t>Subcontractor engagement varies with project complexity</t>
+    <t>Based on OEM supply chain cycle</t>
   </si>
   <si>
-    <t>System Scaffolding Supplies</t>
+    <t>Generators and Inverters</t>
   </si>
   <si>
-    <t>Dependable supply driven by steady demand for construction</t>
+    <t>Power systems included in customization</t>
   </si>
   <si>
-    <t>Usage frequency depends on project scale</t>
+    <t>Regular procurement cycle for power systems</t>
   </si>
   <si>
-    <t>Transportation and Logistics</t>
+    <t>Interior Custom Fittings</t>
   </si>
   <si>
-    <t>Fleet operations supporting material movement</t>
+    <t>Interior fittings for customer specifications</t>
   </si>
   <si>
-    <t>Regular monthly shipment schedules</t>
+    <t>Demands spike during fleet upgrades</t>
   </si>
   <si>
-    <t>Safety and Compliance Checks</t>
+    <t>HVAC Systems</t>
   </si>
   <si>
-    <t>Ongoing compliance with training and inspections</t>
+    <t>Climate control systems included in up-fits</t>
   </si>
   <si>
-    <t>Frequent checks due to regulatory requirements</t>
+    <t>Seasonal increases expected</t>
   </si>
   <si>
     <t>Unit Employees</t>
@@ -259,43 +259,43 @@
     <t>Notes</t>
   </si>
   <si>
-    <t>Scaffold Installer</t>
+    <t>CEO</t>
+  </si>
+  <si>
+    <t>salary</t>
+  </si>
+  <si>
+    <t>Role to be filled post-retirement of current CEO</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Sales Manager</t>
+  </si>
+  <si>
+    <t>Critical for maintaining and expanding client relationships</t>
+  </si>
+  <si>
+    <t>Electrician</t>
   </si>
   <si>
     <t>hourly</t>
   </si>
   <si>
-    <t>Large workforce due to industry standards</t>
+    <t>Essential for fulfilling vehicle modification orders</t>
   </si>
   <si>
-    <t xml:space="preserve"> </t>
+    <t>Production Worker</t>
   </si>
   <si>
-    <t>Site Foreman</t>
+    <t>Perform critical task in vehicle assembly</t>
   </si>
   <si>
-    <t>Foreman to oversee different project sites</t>
+    <t>Office Administrator</t>
   </si>
   <si>
-    <t>Safety Officer</t>
-  </si>
-  <si>
-    <t>In charge of safety training and compliance</t>
-  </si>
-  <si>
-    <t>Administrative Assistant</t>
-  </si>
-  <si>
-    <t>salary</t>
-  </si>
-  <si>
-    <t>Supports company administration and coordination</t>
-  </si>
-  <si>
-    <t>Branch Manager</t>
-  </si>
-  <si>
-    <t>Branch manager for each operational location</t>
+    <t>Support role with administrative functions</t>
   </si>
   <si>
     <t>Sources</t>
@@ -325,40 +325,37 @@
     <t>Notes/Assumptions</t>
   </si>
   <si>
-    <t>Marketing and Advertising</t>
+    <t>Office Rent</t>
   </si>
   <si>
-    <t>Annually</t>
+    <t>Annual</t>
   </si>
   <si>
-    <t>Annual marketing efforts to increase in awareness in newer markets</t>
+    <t>Leases related property for operations</t>
   </si>
   <si>
-    <t>Utility Costs</t>
+    <t>Insurance</t>
   </si>
   <si>
-    <t>Monthly</t>
+    <t>Insurance essential for operational risk management</t>
   </si>
   <si>
-    <t>Estimated based on operation scale</t>
+    <t>IT Services</t>
   </si>
   <si>
-    <t>General Office Supply</t>
+    <t>Ongoing digital infrastructure maintenance</t>
   </si>
   <si>
-    <t>Ongoing operational need for office supplies</t>
+    <t>Utilities</t>
   </si>
   <si>
-    <t>Vehicle Maintenance</t>
+    <t>Yearly utility bills necessary for manufacturing facilities</t>
   </si>
   <si>
-    <t>Consistent spending required for maintenance of transportation fleet</t>
+    <t>Advertising</t>
   </si>
   <si>
-    <t>Professional Fees</t>
-  </si>
-  <si>
-    <t>Legal consulting and audit-related charges</t>
+    <t>Promotional activities to attract and retain clients</t>
   </si>
   <si>
     <t>Capital Expenditures</t>
@@ -370,34 +367,34 @@
     <t>Purchase Date</t>
   </si>
   <si>
-    <t>Scaffold Inventory Enhancement</t>
+    <t>Vehicle Customization Equipment</t>
   </si>
   <si>
-    <t>Expansion and refurbishment of scaffolding stock</t>
+    <t>Equipment required for up-fitting niche vehicles as described in Page 9</t>
   </si>
   <si>
-    <t>Office Equipment Modernization</t>
+    <t>Facility Maintenance</t>
   </si>
   <si>
-    <t>Upgrade office tech to improve efficiency</t>
+    <t>Maintaining and updating the facility leased, as indicated in Page 6</t>
   </si>
   <si>
-    <t>Facilities Expansion</t>
+    <t>IT Infrastructure</t>
   </si>
   <si>
-    <t>Expanding physical infrastructure to support business growth</t>
+    <t>Upgrading IT systems to improve inventory and order processing efficiency</t>
   </si>
   <si>
-    <t>New IT Systems</t>
+    <t>Employee Training Facilities</t>
   </si>
   <si>
-    <t>New software systems to enhance operational efficiency</t>
+    <t>Establishment of facilities for training staff as part of growth</t>
   </si>
   <si>
-    <t>Heavy Equipment Purchase</t>
+    <t>Machinery for Production Line</t>
   </si>
   <si>
-    <t>Ongoing need for specialty equipment for varied projects</t>
+    <t>Necessary for maintaining production as demand increases; Page 9 highlights the growth phase</t>
   </si>
   <si>
     <t>Depreciation Calculations</t>
@@ -514,37 +511,31 @@
     <t>Source Date</t>
   </si>
   <si>
-    <t>BrandSafway</t>
+    <t>Spartan Upfit Services</t>
   </si>
   <si>
-    <t>Market Intelligence</t>
+    <t>-</t>
   </si>
   <si>
-    <t>2023-12-01</t>
+    <t>No Source</t>
   </si>
   <si>
-    <t>Brock Group</t>
+    <t>2023-11-15</t>
   </si>
   <si>
-    <t>Industry Reports</t>
+    <t>ECO Vehicle Systems</t>
   </si>
   <si>
-    <t>PERI Group</t>
+    <t>Utilimaster</t>
   </si>
   <si>
-    <t>Financial Analysis</t>
+    <t>Auto Truck Group</t>
   </si>
   <si>
-    <t>Layher North America</t>
+    <t>Electric Custom Solutions</t>
   </si>
   <si>
-    <t>Competitor Overview</t>
-  </si>
-  <si>
-    <t>Altrad Generation</t>
-  </si>
-  <si>
-    <t>Market Research</t>
+    <t>Industry Overview Page 10</t>
   </si>
   <si>
     <t>Median</t>
@@ -1349,10 +1340,10 @@
         <v>10</v>
       </c>
       <c r="C8" s="7">
-        <v>1000</v>
+        <v>15000</v>
       </c>
       <c r="D8" s="8">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="E8" s="9">
         <f>C$8*D$8</f>
@@ -1365,11 +1356,11 @@
         <v>12</v>
       </c>
       <c r="I8" s="10">
-        <f>HYPERLINK("No source", "Historical data")</f>
+        <f>HYPERLINK("", "Page 9 Custom Up-fitting Description")</f>
         <v>0</v>
       </c>
       <c r="J8" s="10">
-        <f>HYPERLINK("", "Sales forecasts")</f>
+        <f>HYPERLINK("", "Industry Overview Page 10")</f>
         <v>0</v>
       </c>
     </row>
@@ -1381,7 +1372,7 @@
         <v>5000</v>
       </c>
       <c r="D9" s="8">
-        <v>10</v>
+        <v>45</v>
       </c>
       <c r="E9" s="9">
         <f>C$9*D$9</f>
@@ -1394,11 +1385,11 @@
         <v>15</v>
       </c>
       <c r="I9" s="10">
-        <f>HYPERLINK("No source", "Engineering department estimates")</f>
+        <f>HYPERLINK("", "Page 9 Gold Division Overview")</f>
         <v>0</v>
       </c>
       <c r="J9" s="10">
-        <f>HYPERLINK("", "Departmental projections")</f>
+        <f>HYPERLINK("", "No Source")</f>
         <v>0</v>
       </c>
     </row>
@@ -1407,7 +1398,7 @@
         <v>16</v>
       </c>
       <c r="C10" s="7">
-        <v>800</v>
+        <v>1200</v>
       </c>
       <c r="D10" s="8">
         <v>100</v>
@@ -1423,11 +1414,11 @@
         <v>18</v>
       </c>
       <c r="I10" s="10">
-        <f>HYPERLINK("No source", "Market comparison")</f>
+        <f>HYPERLINK("", "Page 9 Product Description")</f>
         <v>0</v>
       </c>
       <c r="J10" s="10">
-        <f>HYPERLINK("", "Inventory system")</f>
+        <f>HYPERLINK("", "No Source")</f>
         <v>0</v>
       </c>
     </row>
@@ -1436,7 +1427,7 @@
         <v>19</v>
       </c>
       <c r="C11" s="7">
-        <v>300</v>
+        <v>2000</v>
       </c>
       <c r="D11" s="8">
         <v>20</v>
@@ -1452,11 +1443,11 @@
         <v>21</v>
       </c>
       <c r="I11" s="10">
-        <f>HYPERLINK("No source", "Course cost analysis")</f>
+        <f>HYPERLINK("", "No Source")</f>
         <v>0</v>
       </c>
       <c r="J11" s="10">
-        <f>HYPERLINK("", "Training department schedule")</f>
+        <f>HYPERLINK("", "Page 14 Consulting Notes")</f>
         <v>0</v>
       </c>
     </row>
@@ -1465,10 +1456,10 @@
         <v>22</v>
       </c>
       <c r="C12" s="7">
-        <v>1500</v>
+        <v>150</v>
       </c>
       <c r="D12" s="8">
-        <v>20</v>
+        <v>200</v>
       </c>
       <c r="E12" s="9">
         <f>C$12*D$12</f>
@@ -1481,11 +1472,11 @@
         <v>24</v>
       </c>
       <c r="I12" s="10">
-        <f>HYPERLINK("No source", "Average bid")</f>
+        <f>HYPERLINK("", "No Source")</f>
         <v>0</v>
       </c>
       <c r="J12" s="10">
-        <f>HYPERLINK("", "Equipment department pipeline")</f>
+        <f>HYPERLINK("", "No Source")</f>
         <v>0</v>
       </c>
     </row>
@@ -1547,10 +1538,10 @@
         <v>31</v>
       </c>
       <c r="C18" s="7">
-        <v>125</v>
+        <v>500</v>
       </c>
       <c r="D18" s="8">
-        <v>400</v>
+        <v>50</v>
       </c>
       <c r="E18" s="9">
         <f>C$18*D$18</f>
@@ -1563,11 +1554,11 @@
         <v>33</v>
       </c>
       <c r="I18" s="10">
-        <f>HYPERLINK("No Source", "Internal financial documents")</f>
+        <f>HYPERLINK("WWW.IBISWORLD.COM", "Industry Report Page 26")</f>
         <v>0</v>
       </c>
       <c r="J18" s="10">
-        <f>HYPERLINK("", "Procurement reports")</f>
+        <f>HYPERLINK("WWW.IBISWORLD.COM", "Industry Report Page 26")</f>
         <v>0</v>
       </c>
     </row>
@@ -1576,10 +1567,10 @@
         <v>34</v>
       </c>
       <c r="C19" s="7">
-        <v>200</v>
+        <v>300</v>
       </c>
       <c r="D19" s="8">
-        <v>50</v>
+        <v>120</v>
       </c>
       <c r="E19" s="9">
         <f>C$19*D$19</f>
@@ -1592,11 +1583,11 @@
         <v>36</v>
       </c>
       <c r="I19" s="10">
-        <f>HYPERLINK("No Source", "Labor contracts")</f>
+        <f>HYPERLINK("", "No Source")</f>
         <v>0</v>
       </c>
       <c r="J19" s="10">
-        <f>HYPERLINK("", "Project management system")</f>
+        <f>HYPERLINK("", "No Source")</f>
         <v>0</v>
       </c>
     </row>
@@ -1605,10 +1596,10 @@
         <v>37</v>
       </c>
       <c r="C20" s="7">
-        <v>80</v>
+        <v>1200</v>
       </c>
       <c r="D20" s="8">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="E20" s="9">
         <f>C$20*D$20</f>
@@ -1621,11 +1612,11 @@
         <v>39</v>
       </c>
       <c r="I20" s="10">
-        <f>HYPERLINK("No Source", "Supplier invoices")</f>
+        <f>HYPERLINK("", "No Source")</f>
         <v>0</v>
       </c>
       <c r="J20" s="10">
-        <f>HYPERLINK("", "Logistics data")</f>
+        <f>HYPERLINK("", "No Source")</f>
         <v>0</v>
       </c>
     </row>
@@ -1634,10 +1625,10 @@
         <v>40</v>
       </c>
       <c r="C21" s="7">
-        <v>150</v>
+        <v>700</v>
       </c>
       <c r="D21" s="8">
-        <v>100</v>
+        <v>40</v>
       </c>
       <c r="E21" s="9">
         <f>C$21*D$21</f>
@@ -1650,11 +1641,11 @@
         <v>42</v>
       </c>
       <c r="I21" s="10">
-        <f>HYPERLINK("No Source", "Transportation agreements")</f>
+        <f>HYPERLINK("", "No Source")</f>
         <v>0</v>
       </c>
       <c r="J21" s="10">
-        <f>HYPERLINK("", "Logistics coordinator input")</f>
+        <f>HYPERLINK("", "No Source")</f>
         <v>0</v>
       </c>
     </row>
@@ -1663,10 +1654,10 @@
         <v>43</v>
       </c>
       <c r="C22" s="7">
-        <v>20</v>
+        <v>800</v>
       </c>
       <c r="D22" s="8">
-        <v>300</v>
+        <v>25</v>
       </c>
       <c r="E22" s="9">
         <f>C$22*D$22</f>
@@ -1679,11 +1670,11 @@
         <v>45</v>
       </c>
       <c r="I22" s="10">
-        <f>HYPERLINK("No Source", "Safety compliance records")</f>
+        <f>HYPERLINK("", "No Source")</f>
         <v>0</v>
       </c>
       <c r="J22" s="10">
-        <f>HYPERLINK("", "Compliance officer reports")</f>
+        <f>HYPERLINK("", "No Source")</f>
         <v>0</v>
       </c>
     </row>
@@ -1716,7 +1707,7 @@
   <sheetData>
     <row r="2" spans="2:7">
       <c r="B2" s="1" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
     </row>
     <row r="3" spans="2:7" ht="5" customHeight="1">
@@ -1729,24 +1720,24 @@
     </row>
     <row r="5" spans="2:7">
       <c r="B5" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="E5" s="4" t="s">
         <v>184</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="F5" s="4" t="s">
         <v>185</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>186</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>187</v>
-      </c>
-      <c r="F5" s="4" t="s">
-        <v>188</v>
       </c>
     </row>
     <row r="6" spans="2:7">
       <c r="B6" s="6" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="C6" s="6" t="s">
         <v>10</v>
@@ -1758,12 +1749,12 @@
         <v>5</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
     </row>
     <row r="7" spans="2:7">
       <c r="B7" s="6" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="C7" s="6" t="s">
         <v>13</v>
@@ -1775,12 +1766,12 @@
         <v>5</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
     </row>
     <row r="8" spans="2:7">
       <c r="B8" s="6" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="C8" s="6" t="s">
         <v>16</v>
@@ -1792,12 +1783,12 @@
         <v>5</v>
       </c>
       <c r="F8" s="6" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="9" spans="2:7">
       <c r="B9" s="6" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="C9" s="6" t="s">
         <v>19</v>
@@ -1809,12 +1800,12 @@
         <v>5</v>
       </c>
       <c r="F9" s="6" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
     </row>
     <row r="10" spans="2:7">
       <c r="B10" s="6" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="C10" s="6" t="s">
         <v>22</v>
@@ -1826,15 +1817,15 @@
         <v>5</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
     </row>
     <row r="11" spans="2:7">
       <c r="B11" s="6" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D11" s="6">
         <v>13</v>
@@ -1843,12 +1834,12 @@
         <v>6</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
     </row>
     <row r="12" spans="2:7">
       <c r="B12" s="6" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="C12" s="6" t="s">
         <v>31</v>
@@ -1860,12 +1851,12 @@
         <v>5</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
     </row>
     <row r="13" spans="2:7">
       <c r="B13" s="6" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="C13" s="6" t="s">
         <v>34</v>
@@ -1877,12 +1868,12 @@
         <v>5</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
     </row>
     <row r="14" spans="2:7">
       <c r="B14" s="6" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="C14" s="6" t="s">
         <v>37</v>
@@ -1894,12 +1885,12 @@
         <v>5</v>
       </c>
       <c r="F14" s="6" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
     </row>
     <row r="15" spans="2:7">
       <c r="B15" s="6" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="C15" s="6" t="s">
         <v>40</v>
@@ -1911,12 +1902,12 @@
         <v>5</v>
       </c>
       <c r="F15" s="6" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
     </row>
     <row r="16" spans="2:7">
       <c r="B16" s="6" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="C16" s="6" t="s">
         <v>43</v>
@@ -1928,15 +1919,15 @@
         <v>5</v>
       </c>
       <c r="F16" s="6" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
     </row>
     <row r="17" spans="2:6">
       <c r="B17" s="6" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="D17" s="6">
         <v>23</v>
@@ -1945,7 +1936,7 @@
         <v>6</v>
       </c>
       <c r="F17" s="6" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
     </row>
     <row r="18" spans="2:6">
@@ -1953,7 +1944,7 @@
         <v>46</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="D18" s="6">
         <v>7</v>
@@ -1962,7 +1953,7 @@
         <v>11</v>
       </c>
       <c r="F18" s="6" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
     </row>
     <row r="19" spans="2:6">
@@ -1970,7 +1961,7 @@
         <v>46</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="D19" s="6">
         <v>7</v>
@@ -1979,7 +1970,7 @@
         <v>11</v>
       </c>
       <c r="F19" s="6" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
     </row>
     <row r="20" spans="2:6">
@@ -1987,7 +1978,7 @@
         <v>46</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="D20" s="6">
         <v>14</v>
@@ -1996,15 +1987,15 @@
         <v>23</v>
       </c>
       <c r="F20" s="6" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
     </row>
     <row r="21" spans="2:6">
       <c r="B21" s="6" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="D21" s="6">
         <v>6</v>
@@ -2013,15 +2004,15 @@
         <v>9</v>
       </c>
       <c r="F21" s="6" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
     </row>
     <row r="22" spans="2:6">
       <c r="B22" s="6" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="D22" s="6">
         <v>13</v>
@@ -2030,15 +2021,15 @@
         <v>21</v>
       </c>
       <c r="F22" s="6" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
     </row>
     <row r="23" spans="2:6">
       <c r="B23" s="6" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="D23" s="6">
         <v>22</v>
@@ -2047,15 +2038,15 @@
         <v>21</v>
       </c>
       <c r="F23" s="6" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
     </row>
     <row r="24" spans="2:6">
       <c r="B24" s="6" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D24" s="6">
         <v>31</v>
@@ -2064,15 +2055,15 @@
         <v>21</v>
       </c>
       <c r="F24" s="6" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
     </row>
     <row r="25" spans="2:6">
       <c r="B25" s="6" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="D25" s="6">
         <v>6</v>
@@ -2081,15 +2072,15 @@
         <v>3</v>
       </c>
       <c r="F25" s="6" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
     </row>
     <row r="26" spans="2:6">
       <c r="B26" s="6" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D26" s="6">
         <v>13</v>
@@ -2098,15 +2089,15 @@
         <v>5</v>
       </c>
       <c r="F26" s="6" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
     </row>
     <row r="27" spans="2:6">
       <c r="B27" s="6" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D27" s="6">
         <v>21</v>
@@ -2115,15 +2106,15 @@
         <v>5</v>
       </c>
       <c r="F27" s="6" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
     </row>
     <row r="28" spans="2:6">
       <c r="B28" s="6" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D28" s="6">
         <v>23</v>
@@ -2132,15 +2123,15 @@
         <v>5</v>
       </c>
       <c r="F28" s="6" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
     </row>
     <row r="29" spans="2:6">
       <c r="B29" s="6" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="C29" s="6" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="D29" s="6">
         <v>26</v>
@@ -2149,15 +2140,15 @@
         <v>5</v>
       </c>
       <c r="F29" s="6" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
     </row>
     <row r="30" spans="2:6">
       <c r="B30" s="6" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="C30" s="6" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D30" s="6">
         <v>27</v>
@@ -2166,15 +2157,15 @@
         <v>5</v>
       </c>
       <c r="F30" s="6" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
     </row>
     <row r="31" spans="2:6">
       <c r="B31" s="6" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="C31" s="6" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D31" s="6">
         <v>28</v>
@@ -2183,15 +2174,15 @@
         <v>5</v>
       </c>
       <c r="F31" s="6" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
     </row>
     <row r="32" spans="2:6">
       <c r="B32" s="6" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="C32" s="6" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D32" s="6">
         <v>29</v>
@@ -2200,15 +2191,15 @@
         <v>5</v>
       </c>
       <c r="F32" s="6" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
     </row>
     <row r="33" spans="2:6">
       <c r="B33" s="6" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="C33" s="6" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D33" s="6">
         <v>32</v>
@@ -2217,15 +2208,15 @@
         <v>5</v>
       </c>
       <c r="F33" s="6" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
     </row>
     <row r="34" spans="2:6">
       <c r="B34" s="6" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="C34" s="6" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D34" s="6">
         <v>33</v>
@@ -2234,15 +2225,15 @@
         <v>5</v>
       </c>
       <c r="F34" s="6" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
     </row>
     <row r="35" spans="2:6">
       <c r="B35" s="6" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="C35" s="6" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D35" s="6">
         <v>36</v>
@@ -2251,15 +2242,15 @@
         <v>5</v>
       </c>
       <c r="F35" s="6" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
     </row>
     <row r="36" spans="2:6">
       <c r="B36" s="6" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="C36" s="6" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D36" s="6">
         <v>37</v>
@@ -2268,15 +2259,15 @@
         <v>5</v>
       </c>
       <c r="F36" s="6" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
     </row>
     <row r="37" spans="2:6">
       <c r="B37" s="6" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="C37" s="6" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="D37" s="6">
         <v>38</v>
@@ -2285,15 +2276,15 @@
         <v>16</v>
       </c>
       <c r="F37" s="6" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
     </row>
     <row r="38" spans="2:6">
       <c r="B38" s="6" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="C38" s="6" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="D38" s="6">
         <v>6</v>
@@ -2302,15 +2293,15 @@
         <v>3</v>
       </c>
       <c r="F38" s="6" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
     </row>
     <row r="39" spans="2:6">
       <c r="B39" s="6" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="C39" s="6" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="D39" s="6">
         <v>6</v>
@@ -2319,15 +2310,15 @@
         <v>2</v>
       </c>
       <c r="F39" s="6" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
     </row>
     <row r="40" spans="2:6">
       <c r="B40" s="6" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="C40" s="6" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="D40" s="6">
         <v>33</v>
@@ -2336,15 +2327,15 @@
         <v>9</v>
       </c>
       <c r="F40" s="6" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
     </row>
     <row r="41" spans="2:6">
       <c r="B41" s="6" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="C41" s="6" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="D41" s="6">
         <v>47</v>
@@ -2353,15 +2344,15 @@
         <v>9</v>
       </c>
       <c r="F41" s="6" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
     </row>
     <row r="42" spans="2:6">
       <c r="B42" s="6" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="C42" s="6" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="D42" s="6">
         <v>61</v>
@@ -2370,15 +2361,15 @@
         <v>9</v>
       </c>
       <c r="F42" s="6" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
     </row>
     <row r="43" spans="2:6">
       <c r="B43" s="6" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="C43" s="6" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="D43" s="6">
         <v>75</v>
@@ -2387,15 +2378,15 @@
         <v>9</v>
       </c>
       <c r="F43" s="6" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
     </row>
     <row r="44" spans="2:6">
       <c r="B44" s="6" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="C44" s="6" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="D44" s="6">
         <v>89</v>
@@ -2404,15 +2395,15 @@
         <v>9</v>
       </c>
       <c r="F44" s="6" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
     </row>
     <row r="45" spans="2:6">
       <c r="B45" s="6" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="C45" s="6" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="D45" s="6">
         <v>103</v>
@@ -2421,15 +2412,15 @@
         <v>9</v>
       </c>
       <c r="F45" s="6" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
     </row>
     <row r="46" spans="2:6">
       <c r="B46" s="6" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="C46" s="6" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="D46" s="6">
         <v>117</v>
@@ -2438,15 +2429,15 @@
         <v>9</v>
       </c>
       <c r="F46" s="6" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
     </row>
     <row r="47" spans="2:6">
       <c r="B47" s="6" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="C47" s="6" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="D47" s="6">
         <v>131</v>
@@ -2455,15 +2446,15 @@
         <v>9</v>
       </c>
       <c r="F47" s="6" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
     </row>
     <row r="48" spans="2:6">
       <c r="B48" s="6" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="C48" s="6" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="D48" s="6">
         <v>145</v>
@@ -2472,15 +2463,15 @@
         <v>9</v>
       </c>
       <c r="F48" s="6" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
     </row>
     <row r="49" spans="2:6">
       <c r="B49" s="6" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="C49" s="6" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="D49" s="6">
         <v>159</v>
@@ -2489,15 +2480,15 @@
         <v>9</v>
       </c>
       <c r="F49" s="6" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
     </row>
     <row r="50" spans="2:6">
       <c r="B50" s="6" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="C50" s="6" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="D50" s="6">
         <v>173</v>
@@ -2506,15 +2497,15 @@
         <v>9</v>
       </c>
       <c r="F50" s="6" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
     </row>
     <row r="51" spans="2:6">
       <c r="B51" s="6" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="C51" s="6" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="D51" s="6">
         <v>6</v>
@@ -2523,15 +2514,15 @@
         <v>3</v>
       </c>
       <c r="F51" s="6" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
     </row>
     <row r="52" spans="2:6">
       <c r="B52" s="6" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="C52" s="6" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="D52" s="6">
         <v>25</v>
@@ -2540,15 +2531,15 @@
         <v>10</v>
       </c>
       <c r="F52" s="6" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
     </row>
     <row r="53" spans="2:6">
       <c r="B53" s="6" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="C53" s="6" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="D53" s="6">
         <v>6</v>
@@ -2557,7 +2548,7 @@
         <v>3</v>
       </c>
       <c r="F53" s="6" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
     </row>
   </sheetData>
@@ -3395,10 +3386,10 @@
         <v>78</v>
       </c>
       <c r="C9" s="8">
-        <v>50</v>
-      </c>
-      <c r="D9" s="14">
-        <v>18</v>
+        <v>1</v>
+      </c>
+      <c r="D9" s="7">
+        <v>130000</v>
       </c>
       <c r="E9" s="8" t="s">
         <v>79</v>
@@ -3942,16 +3933,16 @@
         <v>82</v>
       </c>
       <c r="C10" s="8">
-        <v>10</v>
-      </c>
-      <c r="D10" s="14">
-        <v>25</v>
+        <v>1</v>
+      </c>
+      <c r="D10" s="7">
+        <v>90000</v>
       </c>
       <c r="E10" s="8" t="s">
         <v>79</v>
       </c>
       <c r="F10" s="8">
-        <v>170</v>
+        <v>160</v>
       </c>
       <c r="G10" s="9">
         <f>if(E10="salary",D10/12, F10*D10)</f>
@@ -4489,13 +4480,13 @@
         <v>84</v>
       </c>
       <c r="C11" s="8">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="D11" s="14">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="E11" s="8" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
       <c r="F11" s="8">
         <v>160</v>
@@ -4505,7 +4496,7 @@
         <v>0</v>
       </c>
       <c r="H11" s="6" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="I11" s="6" t="s">
         <v>81</v>
@@ -5033,19 +5024,19 @@
     </row>
     <row r="12" spans="2:142">
       <c r="B12" s="6" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C12" s="8">
-        <v>7</v>
-      </c>
-      <c r="D12" s="7">
-        <v>3000</v>
+        <v>15</v>
+      </c>
+      <c r="D12" s="14">
+        <v>20</v>
       </c>
       <c r="E12" s="8" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="F12" s="8">
-        <v>0</v>
+        <v>160</v>
       </c>
       <c r="G12" s="9">
         <f>if(E12="salary",D12/12, F12*D12)</f>
@@ -5583,16 +5574,16 @@
         <v>89</v>
       </c>
       <c r="C13" s="8">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D13" s="7">
-        <v>6000</v>
+        <v>50000</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="F13" s="8">
-        <v>0</v>
+        <v>160</v>
       </c>
       <c r="G13" s="9">
         <f>if(E13="salary",D13/12, F13*D13)</f>
@@ -6672,7 +6663,7 @@
     </row>
     <row r="21" spans="2:3" ht="10" customHeight="1">
       <c r="B21" s="16" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C21" s="17"/>
     </row>
@@ -6734,7 +6725,7 @@
         <v>95</v>
       </c>
       <c r="I6" s="18">
-        <v>42736</v>
+        <v>40909</v>
       </c>
       <c r="J6" s="18">
         <f>edate(I6,12)</f>
@@ -6773,7 +6764,7 @@
         <v>0</v>
       </c>
       <c r="U6" s="18">
-        <v>42736</v>
+        <v>40909</v>
       </c>
       <c r="V6" s="18">
         <f>edate(U6,1)</f>
@@ -7641,7 +7632,7 @@
         <v>100</v>
       </c>
       <c r="C8" s="7">
-        <v>150000</v>
+        <v>95512</v>
       </c>
       <c r="D8" s="8" t="s">
         <v>101</v>
@@ -8178,13 +8169,13 @@
         <v>103</v>
       </c>
       <c r="C9" s="7">
-        <v>12000</v>
+        <v>34604</v>
       </c>
       <c r="D9" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="F9" s="6" t="s">
         <v>104</v>
-      </c>
-      <c r="F9" s="6" t="s">
-        <v>105</v>
       </c>
       <c r="G9" s="6" t="s">
         <v>81</v>
@@ -8712,16 +8703,16 @@
     </row>
     <row r="10" spans="2:140">
       <c r="B10" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="C10" s="7">
+        <v>25134</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="F10" s="6" t="s">
         <v>106</v>
-      </c>
-      <c r="C10" s="7">
-        <v>2000</v>
-      </c>
-      <c r="D10" s="8" t="s">
-        <v>104</v>
-      </c>
-      <c r="F10" s="6" t="s">
-        <v>107</v>
       </c>
       <c r="G10" s="6" t="s">
         <v>81</v>
@@ -9249,16 +9240,16 @@
     </row>
     <row r="11" spans="2:140">
       <c r="B11" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="C11" s="7">
+        <v>9784</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="F11" s="6" t="s">
         <v>108</v>
-      </c>
-      <c r="C11" s="7">
-        <v>5000</v>
-      </c>
-      <c r="D11" s="8" t="s">
-        <v>104</v>
-      </c>
-      <c r="F11" s="6" t="s">
-        <v>109</v>
       </c>
       <c r="G11" s="6" t="s">
         <v>81</v>
@@ -9786,16 +9777,16 @@
     </row>
     <row r="12" spans="2:140">
       <c r="B12" s="6" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C12" s="7">
-        <v>50000</v>
+        <v>18995</v>
       </c>
       <c r="D12" s="8" t="s">
         <v>101</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G12" s="6" t="s">
         <v>81</v>
@@ -10845,7 +10836,7 @@
     </row>
     <row r="15" spans="2:140">
       <c r="B15" s="3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="16" spans="2:140">
@@ -10856,10 +10847,10 @@
         <v>97</v>
       </c>
       <c r="D16" s="13" t="s">
+        <v>112</v>
+      </c>
+      <c r="E16" s="13" t="s">
         <v>113</v>
-      </c>
-      <c r="E16" s="13" t="s">
-        <v>114</v>
       </c>
       <c r="F16" s="13" t="s">
         <v>99</v>
@@ -10867,19 +10858,19 @@
     </row>
     <row r="17" spans="2:140">
       <c r="B17" s="6" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C17" s="7">
-        <v>750000</v>
+        <v>500000</v>
       </c>
       <c r="D17" s="8">
         <v>10</v>
       </c>
       <c r="E17" s="19">
-        <v>44197</v>
+        <v>45292</v>
       </c>
       <c r="F17" s="6" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="G17" s="6" t="s">
         <v>81</v>
@@ -11407,19 +11398,19 @@
     </row>
     <row r="18" spans="2:140">
       <c r="B18" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="C18" s="7">
+        <v>200000</v>
+      </c>
+      <c r="D18" s="8">
+        <v>20</v>
+      </c>
+      <c r="E18" s="19">
+        <v>45292</v>
+      </c>
+      <c r="F18" s="6" t="s">
         <v>117</v>
-      </c>
-      <c r="C18" s="7">
-        <v>158423</v>
-      </c>
-      <c r="D18" s="8">
-        <v>5</v>
-      </c>
-      <c r="E18" s="19">
-        <v>44197</v>
-      </c>
-      <c r="F18" s="6" t="s">
-        <v>118</v>
       </c>
       <c r="G18" s="6" t="s">
         <v>81</v>
@@ -11947,19 +11938,19 @@
     </row>
     <row r="19" spans="2:140">
       <c r="B19" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="C19" s="7">
+        <v>100000</v>
+      </c>
+      <c r="D19" s="8">
+        <v>5</v>
+      </c>
+      <c r="E19" s="19">
+        <v>45292</v>
+      </c>
+      <c r="F19" s="6" t="s">
         <v>119</v>
-      </c>
-      <c r="C19" s="7">
-        <v>315712</v>
-      </c>
-      <c r="D19" s="8">
-        <v>15</v>
-      </c>
-      <c r="E19" s="19">
-        <v>44197</v>
-      </c>
-      <c r="F19" s="6" t="s">
-        <v>120</v>
       </c>
       <c r="G19" s="6" t="s">
         <v>81</v>
@@ -12487,19 +12478,19 @@
     </row>
     <row r="20" spans="2:140">
       <c r="B20" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="C20" s="7">
+        <v>50000</v>
+      </c>
+      <c r="D20" s="8">
+        <v>10</v>
+      </c>
+      <c r="E20" s="19">
+        <v>45292</v>
+      </c>
+      <c r="F20" s="6" t="s">
         <v>121</v>
-      </c>
-      <c r="C20" s="7">
-        <v>9559</v>
-      </c>
-      <c r="D20" s="8">
-        <v>3</v>
-      </c>
-      <c r="E20" s="19">
-        <v>44197</v>
-      </c>
-      <c r="F20" s="6" t="s">
-        <v>122</v>
       </c>
       <c r="G20" s="6" t="s">
         <v>81</v>
@@ -13027,19 +13018,19 @@
     </row>
     <row r="21" spans="2:140">
       <c r="B21" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="C21" s="7">
+        <v>300000</v>
+      </c>
+      <c r="D21" s="8">
+        <v>8</v>
+      </c>
+      <c r="E21" s="19">
+        <v>45292</v>
+      </c>
+      <c r="F21" s="6" t="s">
         <v>123</v>
-      </c>
-      <c r="C21" s="7">
-        <v>40190</v>
-      </c>
-      <c r="D21" s="8">
-        <v>10</v>
-      </c>
-      <c r="E21" s="19">
-        <v>44197</v>
-      </c>
-      <c r="F21" s="6" t="s">
-        <v>124</v>
       </c>
       <c r="G21" s="6" t="s">
         <v>81</v>
@@ -14089,7 +14080,7 @@
     </row>
     <row r="24" spans="2:140">
       <c r="B24" s="3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="25" spans="2:140">
@@ -14100,18 +14091,18 @@
         <v>97</v>
       </c>
       <c r="D25" s="13" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E25" s="13" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="26" spans="2:140">
       <c r="B26" s="6" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C26" s="7">
-        <v>750000</v>
+        <v>500000</v>
       </c>
       <c r="D26" s="8">
         <v>10</v>
@@ -14643,13 +14634,13 @@
     </row>
     <row r="27" spans="2:140">
       <c r="B27" s="6" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C27" s="7">
-        <v>158423</v>
+        <v>200000</v>
       </c>
       <c r="D27" s="8">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="E27" s="9">
         <f>C27/(D27*12)</f>
@@ -15178,13 +15169,13 @@
     </row>
     <row r="28" spans="2:140">
       <c r="B28" s="6" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C28" s="7">
-        <v>315712</v>
+        <v>100000</v>
       </c>
       <c r="D28" s="8">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="E28" s="9">
         <f>C28/(D28*12)</f>
@@ -15713,13 +15704,13 @@
     </row>
     <row r="29" spans="2:140">
       <c r="B29" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C29" s="7">
-        <v>9559</v>
+        <v>50000</v>
       </c>
       <c r="D29" s="8">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="E29" s="9">
         <f>C29/(D29*12)</f>
@@ -16248,13 +16239,13 @@
     </row>
     <row r="30" spans="2:140">
       <c r="B30" s="6" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C30" s="7">
-        <v>40190</v>
+        <v>300000</v>
       </c>
       <c r="D30" s="8">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E30" s="9">
         <f>C30/(D30*12)</f>
@@ -17322,49 +17313,49 @@
     </row>
     <row r="37" spans="2:3" ht="10" customHeight="1">
       <c r="B37" s="16" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C37" s="17"/>
     </row>
     <row r="38" spans="2:3" ht="10" customHeight="1">
       <c r="B38" s="16" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C38" s="17"/>
     </row>
     <row r="39" spans="2:3" ht="10" customHeight="1">
       <c r="B39" s="16" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C39" s="17"/>
     </row>
     <row r="40" spans="2:3" ht="10" customHeight="1">
       <c r="B40" s="16" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C40" s="17"/>
     </row>
     <row r="41" spans="2:3" ht="10" customHeight="1">
       <c r="B41" s="16" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C41" s="17"/>
     </row>
     <row r="42" spans="2:3" ht="10" customHeight="1">
       <c r="B42" s="16" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C42" s="17"/>
     </row>
     <row r="43" spans="2:3" ht="10" customHeight="1">
       <c r="B43" s="16" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C43" s="17"/>
     </row>
     <row r="44" spans="2:3" ht="10" customHeight="1">
       <c r="B44" s="16" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C44" s="17"/>
     </row>
@@ -17388,7 +17379,7 @@
   <sheetData>
     <row r="2" spans="2:135">
       <c r="B2" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="3" spans="2:135" ht="5" customHeight="1">
@@ -17527,7 +17518,7 @@
     </row>
     <row r="5" spans="2:135">
       <c r="E5" s="3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="P5" s="3" t="s">
         <v>94</v>
@@ -17535,7 +17526,7 @@
     </row>
     <row r="6" spans="2:135">
       <c r="E6" s="18">
-        <v>42736</v>
+        <v>40909</v>
       </c>
       <c r="F6" s="18">
         <f>edate(E6,12)</f>
@@ -17574,7 +17565,7 @@
         <v>0</v>
       </c>
       <c r="P6" s="18">
-        <v>42736</v>
+        <v>40909</v>
       </c>
       <c r="Q6" s="18">
         <f>edate(P6,1)</f>
@@ -18055,7 +18046,7 @@
     </row>
     <row r="7" spans="2:135">
       <c r="B7" s="6" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="P7" s="12" t="s">
         <v>59</v>
@@ -21045,7 +21036,7 @@
     </row>
     <row r="13" spans="2:135">
       <c r="B13" s="3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E13" s="15">
         <f>+E$8+E$9+E$10+E$11+E$12</f>
@@ -21570,7 +21561,7 @@
     </row>
     <row r="14" spans="2:135">
       <c r="B14" s="22" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F14" s="23">
         <f>(F$13-E$13)/E$13</f>
@@ -24672,7 +24663,7 @@
     </row>
     <row r="21" spans="2:135">
       <c r="B21" s="3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E21" s="15">
         <f>+E$16+E$17+E$18+E$19+E$20</f>
@@ -25197,7 +25188,7 @@
     </row>
     <row r="22" spans="2:135">
       <c r="C22" s="24" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E22" s="23">
         <f>E21/E$13</f>
@@ -25722,7 +25713,7 @@
     </row>
     <row r="23" spans="2:135">
       <c r="B23" s="3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E23" s="15">
         <f>+E$13-E$21</f>
@@ -26247,7 +26238,7 @@
     </row>
     <row r="24" spans="2:135">
       <c r="C24" s="24" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E24" s="23">
         <f>E23/E$13</f>
@@ -26772,7 +26763,7 @@
     </row>
     <row r="26" spans="2:135">
       <c r="B26" s="6" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E26" s="9">
         <f>sumif(P6:EE6, E6, P26:EE26)</f>
@@ -27297,7 +27288,7 @@
     </row>
     <row r="27" spans="2:135">
       <c r="B27" s="6" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E27" s="9">
         <f>sumif(P6:EE6, E6, P27:EE27)</f>
@@ -27822,7 +27813,7 @@
     </row>
     <row r="28" spans="2:135">
       <c r="B28" s="6" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E28" s="9">
         <f>sumif(P6:EE6, E6, P28:EE28)</f>
@@ -28227,7 +28218,7 @@
     </row>
     <row r="29" spans="2:135">
       <c r="B29" s="3" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E29" s="15">
         <f>+E$23-E$26-E$27</f>
@@ -28752,7 +28743,7 @@
     </row>
     <row r="30" spans="2:135">
       <c r="C30" s="24" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E30" s="23">
         <f>E29/E$13</f>
@@ -29277,7 +29268,7 @@
     </row>
     <row r="32" spans="2:135">
       <c r="B32" s="6" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E32" s="9">
         <f>sumif(P6:EE6, E6, P32:EE32)</f>
@@ -29802,7 +29793,7 @@
     </row>
     <row r="33" spans="2:135">
       <c r="B33" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E33" s="15">
         <f>+E$29-E$32</f>
@@ -30327,7 +30318,7 @@
     </row>
     <row r="34" spans="2:135">
       <c r="C34" s="24" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E34" s="23">
         <f>E33/E$13</f>
@@ -30852,7 +30843,7 @@
     </row>
     <row r="36" spans="2:135">
       <c r="B36" s="6" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E36" s="9">
         <f>sumif(P6:EE6, E6, P36:EE36)</f>
@@ -31257,7 +31248,7 @@
     </row>
     <row r="37" spans="2:135">
       <c r="B37" s="6" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C37" s="25">
         <v>0.21</v>
@@ -31785,7 +31776,7 @@
     </row>
     <row r="38" spans="2:135">
       <c r="B38" s="3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E38" s="15">
         <f>+E$33-E$36-E$37</f>
@@ -32310,7 +32301,7 @@
     </row>
     <row r="39" spans="2:135">
       <c r="C39" s="24" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E39" s="23">
         <f>E38/E$13</f>
@@ -32854,7 +32845,7 @@
   <sheetData>
     <row r="2" spans="2:135">
       <c r="B2" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="3" spans="2:135" ht="5" customHeight="1">
@@ -33765,7 +33756,7 @@
     </row>
     <row r="8" spans="2:135">
       <c r="B8" s="6" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E8" s="9">
         <f>sumif(P6:EE6, E6, P8:EE8)</f>
@@ -34290,7 +34281,7 @@
     </row>
     <row r="9" spans="2:135">
       <c r="B9" s="6" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E9" s="9">
         <f>sumif(P6:EE6, E6, P9:EE9)</f>
@@ -34815,7 +34806,7 @@
     </row>
     <row r="10" spans="2:135">
       <c r="B10" s="6" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E10" s="9">
         <f>sumif(P6:EE6, E6, P10:EE10)</f>
@@ -35340,37 +35331,37 @@
     </row>
     <row r="11" spans="2:135">
       <c r="B11" s="6" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="12" spans="2:135">
       <c r="B12" s="6" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="13" spans="2:135">
       <c r="B13" s="6" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="14" spans="2:135">
       <c r="B14" s="6" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="15" spans="2:135">
       <c r="B15" s="6" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="16" spans="2:135">
       <c r="B16" s="6" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="17" spans="2:2">
       <c r="B17" s="6" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
   </sheetData>
@@ -35395,7 +35386,7 @@
   <sheetData>
     <row r="2" spans="2:10">
       <c r="B2" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="3" spans="2:10" ht="5" customHeight="1">
@@ -35411,54 +35402,54 @@
     </row>
     <row r="5" spans="2:10">
       <c r="B5" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="C5" s="3" t="s">
         <v>154</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="D5" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="E5" s="3" t="s">
         <v>156</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="F5" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="F5" s="3" t="s">
+      <c r="G5" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="G5" s="3" t="s">
+      <c r="H5" s="3" t="s">
         <v>159</v>
       </c>
-      <c r="H5" s="3" t="s">
+      <c r="I5" s="3" t="s">
         <v>160</v>
       </c>
-      <c r="I5" s="3" t="s">
+      <c r="J5" s="3" t="s">
         <v>161</v>
-      </c>
-      <c r="J5" s="3" t="s">
-        <v>162</v>
       </c>
     </row>
     <row r="6" spans="2:10">
       <c r="B6" s="6" t="s">
+        <v>162</v>
+      </c>
+      <c r="C6" s="26" t="s">
         <v>163</v>
       </c>
-      <c r="C6" s="26">
-        <v>5000</v>
-      </c>
-      <c r="D6" s="26">
-        <v>4000</v>
-      </c>
-      <c r="E6" s="26">
-        <v>500</v>
-      </c>
-      <c r="F6" s="26">
-        <v>1.05</v>
-      </c>
-      <c r="G6" s="26">
-        <v>0.9</v>
-      </c>
-      <c r="H6" s="26">
-        <v>10</v>
+      <c r="D6" s="26" t="s">
+        <v>163</v>
+      </c>
+      <c r="E6" s="26" t="s">
+        <v>163</v>
+      </c>
+      <c r="F6" s="26" t="s">
+        <v>163</v>
+      </c>
+      <c r="G6" s="26" t="s">
+        <v>163</v>
+      </c>
+      <c r="H6" s="26" t="s">
+        <v>163</v>
       </c>
       <c r="I6" s="6" t="s">
         <v>164</v>
@@ -35471,26 +35462,26 @@
       <c r="B7" s="6" t="s">
         <v>166</v>
       </c>
-      <c r="C7" s="26">
-        <v>3000</v>
-      </c>
-      <c r="D7" s="26">
-        <v>2900</v>
-      </c>
-      <c r="E7" s="26">
-        <v>350</v>
-      </c>
-      <c r="F7" s="26">
-        <v>1.1</v>
-      </c>
-      <c r="G7" s="26">
-        <v>0.95</v>
-      </c>
-      <c r="H7" s="26">
-        <v>8</v>
+      <c r="C7" s="26" t="s">
+        <v>163</v>
+      </c>
+      <c r="D7" s="26" t="s">
+        <v>163</v>
+      </c>
+      <c r="E7" s="26" t="s">
+        <v>163</v>
+      </c>
+      <c r="F7" s="26" t="s">
+        <v>163</v>
+      </c>
+      <c r="G7" s="26" t="s">
+        <v>163</v>
+      </c>
+      <c r="H7" s="26" t="s">
+        <v>163</v>
       </c>
       <c r="I7" s="6" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="J7" s="6" t="s">
         <v>165</v>
@@ -35498,28 +35489,28 @@
     </row>
     <row r="8" spans="2:10">
       <c r="B8" s="6" t="s">
-        <v>168</v>
-      </c>
-      <c r="C8" s="26">
-        <v>4500</v>
-      </c>
-      <c r="D8" s="26">
-        <v>4300</v>
-      </c>
-      <c r="E8" s="26">
-        <v>480</v>
-      </c>
-      <c r="F8" s="26">
-        <v>0.98</v>
-      </c>
-      <c r="G8" s="26">
-        <v>0.88</v>
-      </c>
-      <c r="H8" s="26">
-        <v>9</v>
+        <v>167</v>
+      </c>
+      <c r="C8" s="26" t="s">
+        <v>163</v>
+      </c>
+      <c r="D8" s="26" t="s">
+        <v>163</v>
+      </c>
+      <c r="E8" s="26" t="s">
+        <v>163</v>
+      </c>
+      <c r="F8" s="26" t="s">
+        <v>163</v>
+      </c>
+      <c r="G8" s="26" t="s">
+        <v>163</v>
+      </c>
+      <c r="H8" s="26" t="s">
+        <v>163</v>
       </c>
       <c r="I8" s="6" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="J8" s="6" t="s">
         <v>165</v>
@@ -35527,28 +35518,28 @@
     </row>
     <row r="9" spans="2:10">
       <c r="B9" s="6" t="s">
-        <v>170</v>
-      </c>
-      <c r="C9" s="26">
-        <v>3500</v>
-      </c>
-      <c r="D9" s="26">
-        <v>3400</v>
-      </c>
-      <c r="E9" s="26">
-        <v>440</v>
-      </c>
-      <c r="F9" s="26">
-        <v>1.07</v>
-      </c>
-      <c r="G9" s="26">
-        <v>0.92</v>
-      </c>
-      <c r="H9" s="26">
-        <v>11</v>
+        <v>168</v>
+      </c>
+      <c r="C9" s="26" t="s">
+        <v>163</v>
+      </c>
+      <c r="D9" s="26" t="s">
+        <v>163</v>
+      </c>
+      <c r="E9" s="26" t="s">
+        <v>163</v>
+      </c>
+      <c r="F9" s="26" t="s">
+        <v>163</v>
+      </c>
+      <c r="G9" s="26" t="s">
+        <v>163</v>
+      </c>
+      <c r="H9" s="26" t="s">
+        <v>163</v>
       </c>
       <c r="I9" s="6" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="J9" s="6" t="s">
         <v>165</v>
@@ -35556,28 +35547,28 @@
     </row>
     <row r="10" spans="2:10">
       <c r="B10" s="6" t="s">
-        <v>172</v>
-      </c>
-      <c r="C10" s="26">
-        <v>2800</v>
-      </c>
-      <c r="D10" s="26">
-        <v>2700</v>
-      </c>
-      <c r="E10" s="26">
-        <v>390</v>
-      </c>
-      <c r="F10" s="26">
-        <v>1.03</v>
-      </c>
-      <c r="G10" s="26">
-        <v>0.89</v>
-      </c>
-      <c r="H10" s="26">
-        <v>7</v>
+        <v>169</v>
+      </c>
+      <c r="C10" s="26" t="s">
+        <v>163</v>
+      </c>
+      <c r="D10" s="26" t="s">
+        <v>163</v>
+      </c>
+      <c r="E10" s="26" t="s">
+        <v>163</v>
+      </c>
+      <c r="F10" s="26" t="s">
+        <v>163</v>
+      </c>
+      <c r="G10" s="26" t="s">
+        <v>163</v>
+      </c>
+      <c r="H10" s="26" t="s">
+        <v>163</v>
       </c>
       <c r="I10" s="6" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="J10" s="6" t="s">
         <v>165</v>
@@ -35585,7 +35576,7 @@
     </row>
     <row r="11" spans="2:10">
       <c r="B11" s="3" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="C11" s="15">
         <f>MEDIAN(C6:C10)</f>
@@ -35614,7 +35605,7 @@
     </row>
     <row r="12" spans="2:10">
       <c r="B12" s="6" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="C12" s="26">
         <f>AVERAGE(C7:C11)</f>
@@ -35661,7 +35652,7 @@
   <sheetData>
     <row r="2" spans="2:138">
       <c r="B2" s="1" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
     </row>
     <row r="3" spans="2:138" ht="5" customHeight="1">
@@ -35805,12 +35796,12 @@
     </row>
     <row r="5" spans="2:138">
       <c r="I5" s="3" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
     </row>
     <row r="6" spans="2:138">
       <c r="I6" s="18">
-        <v>42736</v>
+        <v>40909</v>
       </c>
       <c r="J6" s="18">
         <f>edate(I6,12)</f>
@@ -35851,20 +35842,20 @@
     </row>
     <row r="8" spans="2:138">
       <c r="B8" s="3" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
     </row>
     <row r="9" spans="2:138">
       <c r="B9" s="4" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
     </row>
     <row r="10" spans="2:138">
       <c r="B10" s="6">
-        <v>2017</v>
+        <v>2012</v>
       </c>
       <c r="C10" s="8">
         <v>1</v>
@@ -35872,7 +35863,7 @@
     </row>
     <row r="11" spans="2:138">
       <c r="B11" s="6">
-        <v>2018</v>
+        <v>2013</v>
       </c>
       <c r="C11" s="8">
         <v>0</v>
@@ -35880,7 +35871,7 @@
     </row>
     <row r="12" spans="2:138">
       <c r="B12" s="6">
-        <v>2019</v>
+        <v>2014</v>
       </c>
       <c r="C12" s="8">
         <v>0</v>
@@ -35888,7 +35879,7 @@
     </row>
     <row r="13" spans="2:138">
       <c r="B13" s="6">
-        <v>2020</v>
+        <v>2015</v>
       </c>
       <c r="C13" s="8">
         <v>0</v>
@@ -35896,7 +35887,7 @@
     </row>
     <row r="14" spans="2:138">
       <c r="B14" s="6">
-        <v>2021</v>
+        <v>2016</v>
       </c>
       <c r="C14" s="8">
         <v>0</v>
@@ -35904,7 +35895,7 @@
     </row>
     <row r="15" spans="2:138">
       <c r="B15" s="6">
-        <v>2022</v>
+        <v>2017</v>
       </c>
       <c r="C15" s="8">
         <v>0</v>
@@ -35912,7 +35903,7 @@
     </row>
     <row r="16" spans="2:138">
       <c r="B16" s="6">
-        <v>2023</v>
+        <v>2018</v>
       </c>
       <c r="C16" s="8">
         <v>0</v>
@@ -35920,7 +35911,7 @@
     </row>
     <row r="17" spans="2:18">
       <c r="B17" s="6">
-        <v>2024</v>
+        <v>2019</v>
       </c>
       <c r="C17" s="8">
         <v>0</v>
@@ -35928,7 +35919,7 @@
     </row>
     <row r="18" spans="2:18">
       <c r="B18" s="6">
-        <v>2025</v>
+        <v>2020</v>
       </c>
       <c r="C18" s="8">
         <v>0</v>
@@ -35936,7 +35927,7 @@
     </row>
     <row r="19" spans="2:18">
       <c r="B19" s="6">
-        <v>2026</v>
+        <v>2021</v>
       </c>
       <c r="C19" s="8">
         <v>0</v>
@@ -35944,7 +35935,7 @@
     </row>
     <row r="21" spans="2:18">
       <c r="B21" s="3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="I21" s="21">
         <f>'Unit_IS'!E$13</f>
@@ -35989,7 +35980,7 @@
     </row>
     <row r="23" spans="2:18">
       <c r="B23" s="6">
-        <v>2017</v>
+        <v>2012</v>
       </c>
       <c r="C23" s="6">
         <f>$C10</f>
@@ -36038,7 +36029,7 @@
     </row>
     <row r="24" spans="2:18">
       <c r="B24" s="6">
-        <v>2018</v>
+        <v>2013</v>
       </c>
       <c r="C24" s="6">
         <f>$C11</f>
@@ -36083,7 +36074,7 @@
     </row>
     <row r="25" spans="2:18">
       <c r="B25" s="6">
-        <v>2019</v>
+        <v>2014</v>
       </c>
       <c r="C25" s="6">
         <f>$C12</f>
@@ -36124,7 +36115,7 @@
     </row>
     <row r="26" spans="2:18">
       <c r="B26" s="6">
-        <v>2020</v>
+        <v>2015</v>
       </c>
       <c r="C26" s="6">
         <f>$C13</f>
@@ -36161,7 +36152,7 @@
     </row>
     <row r="27" spans="2:18">
       <c r="B27" s="6">
-        <v>2021</v>
+        <v>2016</v>
       </c>
       <c r="C27" s="6">
         <f>$C14</f>
@@ -36194,7 +36185,7 @@
     </row>
     <row r="28" spans="2:18">
       <c r="B28" s="6">
-        <v>2022</v>
+        <v>2017</v>
       </c>
       <c r="C28" s="6">
         <f>$C15</f>
@@ -36223,7 +36214,7 @@
     </row>
     <row r="29" spans="2:18">
       <c r="B29" s="6">
-        <v>2023</v>
+        <v>2018</v>
       </c>
       <c r="C29" s="6">
         <f>$C16</f>
@@ -36248,7 +36239,7 @@
     </row>
     <row r="30" spans="2:18">
       <c r="B30" s="6">
-        <v>2024</v>
+        <v>2019</v>
       </c>
       <c r="C30" s="6">
         <f>$C17</f>
@@ -36269,7 +36260,7 @@
     </row>
     <row r="31" spans="2:18">
       <c r="B31" s="6">
-        <v>2025</v>
+        <v>2020</v>
       </c>
       <c r="C31" s="6">
         <f>$C18</f>
@@ -36286,7 +36277,7 @@
     </row>
     <row r="32" spans="2:18">
       <c r="B32" s="6">
-        <v>2026</v>
+        <v>2021</v>
       </c>
       <c r="C32" s="6">
         <f>$C19</f>
@@ -36341,7 +36332,7 @@
     </row>
     <row r="35" spans="2:18">
       <c r="B35" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="I35" s="21">
         <f>'Unit_IS'!E$21</f>
@@ -36386,7 +36377,7 @@
     </row>
     <row r="37" spans="2:18">
       <c r="B37" s="6">
-        <v>2017</v>
+        <v>2012</v>
       </c>
       <c r="C37" s="6">
         <f>$C10</f>
@@ -36435,7 +36426,7 @@
     </row>
     <row r="38" spans="2:18">
       <c r="B38" s="6">
-        <v>2018</v>
+        <v>2013</v>
       </c>
       <c r="C38" s="6">
         <f>$C11</f>
@@ -36480,7 +36471,7 @@
     </row>
     <row r="39" spans="2:18">
       <c r="B39" s="6">
-        <v>2019</v>
+        <v>2014</v>
       </c>
       <c r="C39" s="6">
         <f>$C12</f>
@@ -36521,7 +36512,7 @@
     </row>
     <row r="40" spans="2:18">
       <c r="B40" s="6">
-        <v>2020</v>
+        <v>2015</v>
       </c>
       <c r="C40" s="6">
         <f>$C13</f>
@@ -36558,7 +36549,7 @@
     </row>
     <row r="41" spans="2:18">
       <c r="B41" s="6">
-        <v>2021</v>
+        <v>2016</v>
       </c>
       <c r="C41" s="6">
         <f>$C14</f>
@@ -36591,7 +36582,7 @@
     </row>
     <row r="42" spans="2:18">
       <c r="B42" s="6">
-        <v>2022</v>
+        <v>2017</v>
       </c>
       <c r="C42" s="6">
         <f>$C15</f>
@@ -36620,7 +36611,7 @@
     </row>
     <row r="43" spans="2:18">
       <c r="B43" s="6">
-        <v>2023</v>
+        <v>2018</v>
       </c>
       <c r="C43" s="6">
         <f>$C16</f>
@@ -36645,7 +36636,7 @@
     </row>
     <row r="44" spans="2:18">
       <c r="B44" s="6">
-        <v>2024</v>
+        <v>2019</v>
       </c>
       <c r="C44" s="6">
         <f>$C17</f>
@@ -36666,7 +36657,7 @@
     </row>
     <row r="45" spans="2:18">
       <c r="B45" s="6">
-        <v>2025</v>
+        <v>2020</v>
       </c>
       <c r="C45" s="6">
         <f>$C18</f>
@@ -36683,7 +36674,7 @@
     </row>
     <row r="46" spans="2:18">
       <c r="B46" s="6">
-        <v>2026</v>
+        <v>2021</v>
       </c>
       <c r="C46" s="6">
         <f>$C19</f>
@@ -36738,7 +36729,7 @@
     </row>
     <row r="49" spans="2:18">
       <c r="B49" s="3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="I49" s="21">
         <f>'Unit_IS'!E$23</f>
@@ -36783,7 +36774,7 @@
     </row>
     <row r="51" spans="2:18">
       <c r="B51" s="6">
-        <v>2017</v>
+        <v>2012</v>
       </c>
       <c r="C51" s="6">
         <f>$C10</f>
@@ -36832,7 +36823,7 @@
     </row>
     <row r="52" spans="2:18">
       <c r="B52" s="6">
-        <v>2018</v>
+        <v>2013</v>
       </c>
       <c r="C52" s="6">
         <f>$C11</f>
@@ -36877,7 +36868,7 @@
     </row>
     <row r="53" spans="2:18">
       <c r="B53" s="6">
-        <v>2019</v>
+        <v>2014</v>
       </c>
       <c r="C53" s="6">
         <f>$C12</f>
@@ -36918,7 +36909,7 @@
     </row>
     <row r="54" spans="2:18">
       <c r="B54" s="6">
-        <v>2020</v>
+        <v>2015</v>
       </c>
       <c r="C54" s="6">
         <f>$C13</f>
@@ -36955,7 +36946,7 @@
     </row>
     <row r="55" spans="2:18">
       <c r="B55" s="6">
-        <v>2021</v>
+        <v>2016</v>
       </c>
       <c r="C55" s="6">
         <f>$C14</f>
@@ -36988,7 +36979,7 @@
     </row>
     <row r="56" spans="2:18">
       <c r="B56" s="6">
-        <v>2022</v>
+        <v>2017</v>
       </c>
       <c r="C56" s="6">
         <f>$C15</f>
@@ -37017,7 +37008,7 @@
     </row>
     <row r="57" spans="2:18">
       <c r="B57" s="6">
-        <v>2023</v>
+        <v>2018</v>
       </c>
       <c r="C57" s="6">
         <f>$C16</f>
@@ -37042,7 +37033,7 @@
     </row>
     <row r="58" spans="2:18">
       <c r="B58" s="6">
-        <v>2024</v>
+        <v>2019</v>
       </c>
       <c r="C58" s="6">
         <f>$C17</f>
@@ -37063,7 +37054,7 @@
     </row>
     <row r="59" spans="2:18">
       <c r="B59" s="6">
-        <v>2025</v>
+        <v>2020</v>
       </c>
       <c r="C59" s="6">
         <f>$C18</f>
@@ -37080,7 +37071,7 @@
     </row>
     <row r="60" spans="2:18">
       <c r="B60" s="6">
-        <v>2026</v>
+        <v>2021</v>
       </c>
       <c r="C60" s="6">
         <f>$C19</f>
@@ -37135,7 +37126,7 @@
     </row>
     <row r="63" spans="2:18">
       <c r="B63" s="3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="I63" s="21">
         <f>'Unit_IS'!E$26</f>
@@ -37180,7 +37171,7 @@
     </row>
     <row r="65" spans="2:18">
       <c r="B65" s="6">
-        <v>2017</v>
+        <v>2012</v>
       </c>
       <c r="C65" s="6">
         <f>$C10</f>
@@ -37229,7 +37220,7 @@
     </row>
     <row r="66" spans="2:18">
       <c r="B66" s="6">
-        <v>2018</v>
+        <v>2013</v>
       </c>
       <c r="C66" s="6">
         <f>$C11</f>
@@ -37274,7 +37265,7 @@
     </row>
     <row r="67" spans="2:18">
       <c r="B67" s="6">
-        <v>2019</v>
+        <v>2014</v>
       </c>
       <c r="C67" s="6">
         <f>$C12</f>
@@ -37315,7 +37306,7 @@
     </row>
     <row r="68" spans="2:18">
       <c r="B68" s="6">
-        <v>2020</v>
+        <v>2015</v>
       </c>
       <c r="C68" s="6">
         <f>$C13</f>
@@ -37352,7 +37343,7 @@
     </row>
     <row r="69" spans="2:18">
       <c r="B69" s="6">
-        <v>2021</v>
+        <v>2016</v>
       </c>
       <c r="C69" s="6">
         <f>$C14</f>
@@ -37385,7 +37376,7 @@
     </row>
     <row r="70" spans="2:18">
       <c r="B70" s="6">
-        <v>2022</v>
+        <v>2017</v>
       </c>
       <c r="C70" s="6">
         <f>$C15</f>
@@ -37414,7 +37405,7 @@
     </row>
     <row r="71" spans="2:18">
       <c r="B71" s="6">
-        <v>2023</v>
+        <v>2018</v>
       </c>
       <c r="C71" s="6">
         <f>$C16</f>
@@ -37439,7 +37430,7 @@
     </row>
     <row r="72" spans="2:18">
       <c r="B72" s="6">
-        <v>2024</v>
+        <v>2019</v>
       </c>
       <c r="C72" s="6">
         <f>$C17</f>
@@ -37460,7 +37451,7 @@
     </row>
     <row r="73" spans="2:18">
       <c r="B73" s="6">
-        <v>2025</v>
+        <v>2020</v>
       </c>
       <c r="C73" s="6">
         <f>$C18</f>
@@ -37477,7 +37468,7 @@
     </row>
     <row r="74" spans="2:18">
       <c r="B74" s="6">
-        <v>2026</v>
+        <v>2021</v>
       </c>
       <c r="C74" s="6">
         <f>$C19</f>
@@ -37532,7 +37523,7 @@
     </row>
     <row r="77" spans="2:18">
       <c r="B77" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="I77" s="21">
         <f>'Unit_IS'!E$27</f>
@@ -37577,7 +37568,7 @@
     </row>
     <row r="79" spans="2:18">
       <c r="B79" s="6">
-        <v>2017</v>
+        <v>2012</v>
       </c>
       <c r="C79" s="6">
         <f>$C10</f>
@@ -37626,7 +37617,7 @@
     </row>
     <row r="80" spans="2:18">
       <c r="B80" s="6">
-        <v>2018</v>
+        <v>2013</v>
       </c>
       <c r="C80" s="6">
         <f>$C11</f>
@@ -37671,7 +37662,7 @@
     </row>
     <row r="81" spans="2:18">
       <c r="B81" s="6">
-        <v>2019</v>
+        <v>2014</v>
       </c>
       <c r="C81" s="6">
         <f>$C12</f>
@@ -37712,7 +37703,7 @@
     </row>
     <row r="82" spans="2:18">
       <c r="B82" s="6">
-        <v>2020</v>
+        <v>2015</v>
       </c>
       <c r="C82" s="6">
         <f>$C13</f>
@@ -37749,7 +37740,7 @@
     </row>
     <row r="83" spans="2:18">
       <c r="B83" s="6">
-        <v>2021</v>
+        <v>2016</v>
       </c>
       <c r="C83" s="6">
         <f>$C14</f>
@@ -37782,7 +37773,7 @@
     </row>
     <row r="84" spans="2:18">
       <c r="B84" s="6">
-        <v>2022</v>
+        <v>2017</v>
       </c>
       <c r="C84" s="6">
         <f>$C15</f>
@@ -37811,7 +37802,7 @@
     </row>
     <row r="85" spans="2:18">
       <c r="B85" s="6">
-        <v>2023</v>
+        <v>2018</v>
       </c>
       <c r="C85" s="6">
         <f>$C16</f>
@@ -37836,7 +37827,7 @@
     </row>
     <row r="86" spans="2:18">
       <c r="B86" s="6">
-        <v>2024</v>
+        <v>2019</v>
       </c>
       <c r="C86" s="6">
         <f>$C17</f>
@@ -37857,7 +37848,7 @@
     </row>
     <row r="87" spans="2:18">
       <c r="B87" s="6">
-        <v>2025</v>
+        <v>2020</v>
       </c>
       <c r="C87" s="6">
         <f>$C18</f>
@@ -37874,7 +37865,7 @@
     </row>
     <row r="88" spans="2:18">
       <c r="B88" s="6">
-        <v>2026</v>
+        <v>2021</v>
       </c>
       <c r="C88" s="6">
         <f>$C19</f>
@@ -37929,7 +37920,7 @@
     </row>
     <row r="91" spans="2:18">
       <c r="B91" s="3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="I91" s="21">
         <f>'Unit_IS'!E$28</f>
@@ -37974,7 +37965,7 @@
     </row>
     <row r="93" spans="2:18">
       <c r="B93" s="6">
-        <v>2017</v>
+        <v>2012</v>
       </c>
       <c r="C93" s="6">
         <f>$C10</f>
@@ -38023,7 +38014,7 @@
     </row>
     <row r="94" spans="2:18">
       <c r="B94" s="6">
-        <v>2018</v>
+        <v>2013</v>
       </c>
       <c r="C94" s="6">
         <f>$C11</f>
@@ -38068,7 +38059,7 @@
     </row>
     <row r="95" spans="2:18">
       <c r="B95" s="6">
-        <v>2019</v>
+        <v>2014</v>
       </c>
       <c r="C95" s="6">
         <f>$C12</f>
@@ -38109,7 +38100,7 @@
     </row>
     <row r="96" spans="2:18">
       <c r="B96" s="6">
-        <v>2020</v>
+        <v>2015</v>
       </c>
       <c r="C96" s="6">
         <f>$C13</f>
@@ -38146,7 +38137,7 @@
     </row>
     <row r="97" spans="2:18">
       <c r="B97" s="6">
-        <v>2021</v>
+        <v>2016</v>
       </c>
       <c r="C97" s="6">
         <f>$C14</f>
@@ -38179,7 +38170,7 @@
     </row>
     <row r="98" spans="2:18">
       <c r="B98" s="6">
-        <v>2022</v>
+        <v>2017</v>
       </c>
       <c r="C98" s="6">
         <f>$C15</f>
@@ -38208,7 +38199,7 @@
     </row>
     <row r="99" spans="2:18">
       <c r="B99" s="6">
-        <v>2023</v>
+        <v>2018</v>
       </c>
       <c r="C99" s="6">
         <f>$C16</f>
@@ -38233,7 +38224,7 @@
     </row>
     <row r="100" spans="2:18">
       <c r="B100" s="6">
-        <v>2024</v>
+        <v>2019</v>
       </c>
       <c r="C100" s="6">
         <f>$C17</f>
@@ -38254,7 +38245,7 @@
     </row>
     <row r="101" spans="2:18">
       <c r="B101" s="6">
-        <v>2025</v>
+        <v>2020</v>
       </c>
       <c r="C101" s="6">
         <f>$C18</f>
@@ -38271,7 +38262,7 @@
     </row>
     <row r="102" spans="2:18">
       <c r="B102" s="6">
-        <v>2026</v>
+        <v>2021</v>
       </c>
       <c r="C102" s="6">
         <f>$C19</f>
@@ -38326,7 +38317,7 @@
     </row>
     <row r="105" spans="2:18">
       <c r="B105" s="3" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="I105" s="21">
         <f>'Unit_IS'!E$29</f>
@@ -38371,7 +38362,7 @@
     </row>
     <row r="107" spans="2:18">
       <c r="B107" s="6">
-        <v>2017</v>
+        <v>2012</v>
       </c>
       <c r="C107" s="6">
         <f>$C10</f>
@@ -38420,7 +38411,7 @@
     </row>
     <row r="108" spans="2:18">
       <c r="B108" s="6">
-        <v>2018</v>
+        <v>2013</v>
       </c>
       <c r="C108" s="6">
         <f>$C11</f>
@@ -38465,7 +38456,7 @@
     </row>
     <row r="109" spans="2:18">
       <c r="B109" s="6">
-        <v>2019</v>
+        <v>2014</v>
       </c>
       <c r="C109" s="6">
         <f>$C12</f>
@@ -38506,7 +38497,7 @@
     </row>
     <row r="110" spans="2:18">
       <c r="B110" s="6">
-        <v>2020</v>
+        <v>2015</v>
       </c>
       <c r="C110" s="6">
         <f>$C13</f>
@@ -38543,7 +38534,7 @@
     </row>
     <row r="111" spans="2:18">
       <c r="B111" s="6">
-        <v>2021</v>
+        <v>2016</v>
       </c>
       <c r="C111" s="6">
         <f>$C14</f>
@@ -38576,7 +38567,7 @@
     </row>
     <row r="112" spans="2:18">
       <c r="B112" s="6">
-        <v>2022</v>
+        <v>2017</v>
       </c>
       <c r="C112" s="6">
         <f>$C15</f>
@@ -38605,7 +38596,7 @@
     </row>
     <row r="113" spans="2:18">
       <c r="B113" s="6">
-        <v>2023</v>
+        <v>2018</v>
       </c>
       <c r="C113" s="6">
         <f>$C16</f>
@@ -38630,7 +38621,7 @@
     </row>
     <row r="114" spans="2:18">
       <c r="B114" s="6">
-        <v>2024</v>
+        <v>2019</v>
       </c>
       <c r="C114" s="6">
         <f>$C17</f>
@@ -38651,7 +38642,7 @@
     </row>
     <row r="115" spans="2:18">
       <c r="B115" s="6">
-        <v>2025</v>
+        <v>2020</v>
       </c>
       <c r="C115" s="6">
         <f>$C18</f>
@@ -38668,7 +38659,7 @@
     </row>
     <row r="116" spans="2:18">
       <c r="B116" s="6">
-        <v>2026</v>
+        <v>2021</v>
       </c>
       <c r="C116" s="6">
         <f>$C19</f>
@@ -38723,7 +38714,7 @@
     </row>
     <row r="119" spans="2:18">
       <c r="B119" s="3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="I119" s="21">
         <f>'Unit_IS'!E$32</f>
@@ -38768,7 +38759,7 @@
     </row>
     <row r="121" spans="2:18">
       <c r="B121" s="6">
-        <v>2017</v>
+        <v>2012</v>
       </c>
       <c r="C121" s="6">
         <f>$C10</f>
@@ -38817,7 +38808,7 @@
     </row>
     <row r="122" spans="2:18">
       <c r="B122" s="6">
-        <v>2018</v>
+        <v>2013</v>
       </c>
       <c r="C122" s="6">
         <f>$C11</f>
@@ -38862,7 +38853,7 @@
     </row>
     <row r="123" spans="2:18">
       <c r="B123" s="6">
-        <v>2019</v>
+        <v>2014</v>
       </c>
       <c r="C123" s="6">
         <f>$C12</f>
@@ -38903,7 +38894,7 @@
     </row>
     <row r="124" spans="2:18">
       <c r="B124" s="6">
-        <v>2020</v>
+        <v>2015</v>
       </c>
       <c r="C124" s="6">
         <f>$C13</f>
@@ -38940,7 +38931,7 @@
     </row>
     <row r="125" spans="2:18">
       <c r="B125" s="6">
-        <v>2021</v>
+        <v>2016</v>
       </c>
       <c r="C125" s="6">
         <f>$C14</f>
@@ -38973,7 +38964,7 @@
     </row>
     <row r="126" spans="2:18">
       <c r="B126" s="6">
-        <v>2022</v>
+        <v>2017</v>
       </c>
       <c r="C126" s="6">
         <f>$C15</f>
@@ -39002,7 +38993,7 @@
     </row>
     <row r="127" spans="2:18">
       <c r="B127" s="6">
-        <v>2023</v>
+        <v>2018</v>
       </c>
       <c r="C127" s="6">
         <f>$C16</f>
@@ -39027,7 +39018,7 @@
     </row>
     <row r="128" spans="2:18">
       <c r="B128" s="6">
-        <v>2024</v>
+        <v>2019</v>
       </c>
       <c r="C128" s="6">
         <f>$C17</f>
@@ -39048,7 +39039,7 @@
     </row>
     <row r="129" spans="2:18">
       <c r="B129" s="6">
-        <v>2025</v>
+        <v>2020</v>
       </c>
       <c r="C129" s="6">
         <f>$C18</f>
@@ -39065,7 +39056,7 @@
     </row>
     <row r="130" spans="2:18">
       <c r="B130" s="6">
-        <v>2026</v>
+        <v>2021</v>
       </c>
       <c r="C130" s="6">
         <f>$C19</f>
@@ -39120,7 +39111,7 @@
     </row>
     <row r="133" spans="2:18">
       <c r="B133" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="I133" s="21">
         <f>'Unit_IS'!E$33</f>
@@ -39165,7 +39156,7 @@
     </row>
     <row r="135" spans="2:18">
       <c r="B135" s="6">
-        <v>2017</v>
+        <v>2012</v>
       </c>
       <c r="C135" s="6">
         <f>$C10</f>
@@ -39214,7 +39205,7 @@
     </row>
     <row r="136" spans="2:18">
       <c r="B136" s="6">
-        <v>2018</v>
+        <v>2013</v>
       </c>
       <c r="C136" s="6">
         <f>$C11</f>
@@ -39259,7 +39250,7 @@
     </row>
     <row r="137" spans="2:18">
       <c r="B137" s="6">
-        <v>2019</v>
+        <v>2014</v>
       </c>
       <c r="C137" s="6">
         <f>$C12</f>
@@ -39300,7 +39291,7 @@
     </row>
     <row r="138" spans="2:18">
       <c r="B138" s="6">
-        <v>2020</v>
+        <v>2015</v>
       </c>
       <c r="C138" s="6">
         <f>$C13</f>
@@ -39337,7 +39328,7 @@
     </row>
     <row r="139" spans="2:18">
       <c r="B139" s="6">
-        <v>2021</v>
+        <v>2016</v>
       </c>
       <c r="C139" s="6">
         <f>$C14</f>
@@ -39370,7 +39361,7 @@
     </row>
     <row r="140" spans="2:18">
       <c r="B140" s="6">
-        <v>2022</v>
+        <v>2017</v>
       </c>
       <c r="C140" s="6">
         <f>$C15</f>
@@ -39399,7 +39390,7 @@
     </row>
     <row r="141" spans="2:18">
       <c r="B141" s="6">
-        <v>2023</v>
+        <v>2018</v>
       </c>
       <c r="C141" s="6">
         <f>$C16</f>
@@ -39424,7 +39415,7 @@
     </row>
     <row r="142" spans="2:18">
       <c r="B142" s="6">
-        <v>2024</v>
+        <v>2019</v>
       </c>
       <c r="C142" s="6">
         <f>$C17</f>
@@ -39445,7 +39436,7 @@
     </row>
     <row r="143" spans="2:18">
       <c r="B143" s="6">
-        <v>2025</v>
+        <v>2020</v>
       </c>
       <c r="C143" s="6">
         <f>$C18</f>
@@ -39462,7 +39453,7 @@
     </row>
     <row r="144" spans="2:18">
       <c r="B144" s="6">
-        <v>2026</v>
+        <v>2021</v>
       </c>
       <c r="C144" s="6">
         <f>$C19</f>
@@ -39517,7 +39508,7 @@
     </row>
     <row r="147" spans="2:18">
       <c r="B147" s="3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="I147" s="21">
         <f>'Unit_IS'!E$36</f>
@@ -39562,7 +39553,7 @@
     </row>
     <row r="149" spans="2:18">
       <c r="B149" s="6">
-        <v>2017</v>
+        <v>2012</v>
       </c>
       <c r="C149" s="6">
         <f>$C10</f>
@@ -39611,7 +39602,7 @@
     </row>
     <row r="150" spans="2:18">
       <c r="B150" s="6">
-        <v>2018</v>
+        <v>2013</v>
       </c>
       <c r="C150" s="6">
         <f>$C11</f>
@@ -39656,7 +39647,7 @@
     </row>
     <row r="151" spans="2:18">
       <c r="B151" s="6">
-        <v>2019</v>
+        <v>2014</v>
       </c>
       <c r="C151" s="6">
         <f>$C12</f>
@@ -39697,7 +39688,7 @@
     </row>
     <row r="152" spans="2:18">
       <c r="B152" s="6">
-        <v>2020</v>
+        <v>2015</v>
       </c>
       <c r="C152" s="6">
         <f>$C13</f>
@@ -39734,7 +39725,7 @@
     </row>
     <row r="153" spans="2:18">
       <c r="B153" s="6">
-        <v>2021</v>
+        <v>2016</v>
       </c>
       <c r="C153" s="6">
         <f>$C14</f>
@@ -39767,7 +39758,7 @@
     </row>
     <row r="154" spans="2:18">
       <c r="B154" s="6">
-        <v>2022</v>
+        <v>2017</v>
       </c>
       <c r="C154" s="6">
         <f>$C15</f>
@@ -39796,7 +39787,7 @@
     </row>
     <row r="155" spans="2:18">
       <c r="B155" s="6">
-        <v>2023</v>
+        <v>2018</v>
       </c>
       <c r="C155" s="6">
         <f>$C16</f>
@@ -39821,7 +39812,7 @@
     </row>
     <row r="156" spans="2:18">
       <c r="B156" s="6">
-        <v>2024</v>
+        <v>2019</v>
       </c>
       <c r="C156" s="6">
         <f>$C17</f>
@@ -39842,7 +39833,7 @@
     </row>
     <row r="157" spans="2:18">
       <c r="B157" s="6">
-        <v>2025</v>
+        <v>2020</v>
       </c>
       <c r="C157" s="6">
         <f>$C18</f>
@@ -39859,7 +39850,7 @@
     </row>
     <row r="158" spans="2:18">
       <c r="B158" s="6">
-        <v>2026</v>
+        <v>2021</v>
       </c>
       <c r="C158" s="6">
         <f>$C19</f>
@@ -39914,7 +39905,7 @@
     </row>
     <row r="161" spans="2:18">
       <c r="B161" s="3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="I161" s="21">
         <f>'Unit_IS'!P$38</f>
@@ -39959,7 +39950,7 @@
     </row>
     <row r="163" spans="2:18">
       <c r="B163" s="6">
-        <v>2017</v>
+        <v>2012</v>
       </c>
       <c r="C163" s="6">
         <f>$C10</f>
@@ -40008,7 +39999,7 @@
     </row>
     <row r="164" spans="2:18">
       <c r="B164" s="6">
-        <v>2018</v>
+        <v>2013</v>
       </c>
       <c r="C164" s="6">
         <f>$C11</f>
@@ -40053,7 +40044,7 @@
     </row>
     <row r="165" spans="2:18">
       <c r="B165" s="6">
-        <v>2019</v>
+        <v>2014</v>
       </c>
       <c r="C165" s="6">
         <f>$C12</f>
@@ -40094,7 +40085,7 @@
     </row>
     <row r="166" spans="2:18">
       <c r="B166" s="6">
-        <v>2020</v>
+        <v>2015</v>
       </c>
       <c r="C166" s="6">
         <f>$C13</f>
@@ -40131,7 +40122,7 @@
     </row>
     <row r="167" spans="2:18">
       <c r="B167" s="6">
-        <v>2021</v>
+        <v>2016</v>
       </c>
       <c r="C167" s="6">
         <f>$C14</f>
@@ -40164,7 +40155,7 @@
     </row>
     <row r="168" spans="2:18">
       <c r="B168" s="6">
-        <v>2022</v>
+        <v>2017</v>
       </c>
       <c r="C168" s="6">
         <f>$C15</f>
@@ -40193,7 +40184,7 @@
     </row>
     <row r="169" spans="2:18">
       <c r="B169" s="6">
-        <v>2023</v>
+        <v>2018</v>
       </c>
       <c r="C169" s="6">
         <f>$C16</f>
@@ -40218,7 +40209,7 @@
     </row>
     <row r="170" spans="2:18">
       <c r="B170" s="6">
-        <v>2024</v>
+        <v>2019</v>
       </c>
       <c r="C170" s="6">
         <f>$C17</f>
@@ -40239,7 +40230,7 @@
     </row>
     <row r="171" spans="2:18">
       <c r="B171" s="6">
-        <v>2025</v>
+        <v>2020</v>
       </c>
       <c r="C171" s="6">
         <f>$C18</f>
@@ -40256,7 +40247,7 @@
     </row>
     <row r="172" spans="2:18">
       <c r="B172" s="6">
-        <v>2026</v>
+        <v>2021</v>
       </c>
       <c r="C172" s="6">
         <f>$C19</f>
@@ -40329,7 +40320,7 @@
   <sheetData>
     <row r="2" spans="2:19">
       <c r="B2" s="1" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
     </row>
     <row r="3" spans="2:19" ht="5" customHeight="1">
@@ -40354,7 +40345,7 @@
     </row>
     <row r="5" spans="2:19">
       <c r="E5" s="3" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="J5" s="3" t="s">
         <v>93</v>
@@ -40362,7 +40353,7 @@
     </row>
     <row r="6" spans="2:19">
       <c r="J6" s="18">
-        <v>42736</v>
+        <v>40909</v>
       </c>
       <c r="K6" s="18">
         <f>edate(J6,12)</f>
@@ -40403,7 +40394,7 @@
     </row>
     <row r="8" spans="2:19">
       <c r="B8" s="6" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="J8" s="21">
         <f>'Roll Out'!I$33</f>
@@ -40448,7 +40439,7 @@
     </row>
     <row r="9" spans="2:19">
       <c r="B9" s="6" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="J9" s="21">
         <f>'Roll Out'!I$47</f>
@@ -40493,7 +40484,7 @@
     </row>
     <row r="10" spans="2:19">
       <c r="B10" s="3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="J10" s="15">
         <f>+J$8-J$9</f>
@@ -40538,7 +40529,7 @@
     </row>
     <row r="11" spans="2:19">
       <c r="C11" s="24" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="J11" s="23">
         <f>J10/J$8</f>
@@ -40583,7 +40574,7 @@
     </row>
     <row r="13" spans="2:19">
       <c r="B13" s="6" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="J13" s="21">
         <f>'Roll Out'!I$75</f>
@@ -40628,7 +40619,7 @@
     </row>
     <row r="14" spans="2:19">
       <c r="B14" s="6" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="J14" s="21">
         <f>'Roll Out'!I$89</f>
@@ -40673,12 +40664,12 @@
     </row>
     <row r="15" spans="2:19">
       <c r="B15" s="6" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="16" spans="2:19">
       <c r="B16" s="3" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="J16" s="15">
         <f>+J$10-J$13-J$14</f>
@@ -40723,7 +40714,7 @@
     </row>
     <row r="17" spans="2:19">
       <c r="C17" s="24" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="J17" s="23">
         <f>J16/J$8</f>
@@ -40768,7 +40759,7 @@
     </row>
     <row r="19" spans="2:19">
       <c r="B19" s="6" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="J19" s="21">
         <f>'Roll Out'!I$131</f>
@@ -40813,7 +40804,7 @@
     </row>
     <row r="20" spans="2:19">
       <c r="B20" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="J20" s="15">
         <f>+J$16-J$19</f>
@@ -40858,7 +40849,7 @@
     </row>
     <row r="21" spans="2:19">
       <c r="C21" s="24" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="J21" s="23">
         <f>J20/J$8</f>
@@ -40903,7 +40894,7 @@
     </row>
     <row r="23" spans="2:19">
       <c r="B23" s="6" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="J23" s="21">
         <f>'Roll Out'!I$159</f>
@@ -40948,7 +40939,7 @@
     </row>
     <row r="24" spans="2:19">
       <c r="B24" s="6" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C24" s="25">
         <v>0.21</v>
@@ -40996,7 +40987,7 @@
     </row>
     <row r="25" spans="2:19">
       <c r="B25" s="3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="J25" s="15">
         <f>+J$20-J$23-J$24</f>
@@ -41041,7 +41032,7 @@
     </row>
     <row r="26" spans="2:19">
       <c r="C26" s="24" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="J26" s="23">
         <f>J25/J$8</f>
@@ -41104,7 +41095,7 @@
   <sheetData>
     <row r="2" spans="2:135">
       <c r="B2" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="3" spans="2:135" ht="5" customHeight="1">
@@ -42015,7 +42006,7 @@
     </row>
     <row r="8" spans="2:135">
       <c r="B8" s="6" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E8" s="9">
         <f>sumif(P6:EE6, E6, P8:EE8)</f>
@@ -42540,7 +42531,7 @@
     </row>
     <row r="9" spans="2:135">
       <c r="B9" s="6" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E9" s="9">
         <f>sumif(P6:EE6, E6, P9:EE9)</f>
@@ -43065,7 +43056,7 @@
     </row>
     <row r="10" spans="2:135">
       <c r="B10" s="6" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E10" s="9">
         <f>sumif(P6:EE6, E6, P10:EE10)</f>
@@ -43590,37 +43581,37 @@
     </row>
     <row r="11" spans="2:135">
       <c r="B11" s="6" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="12" spans="2:135">
       <c r="B12" s="6" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="13" spans="2:135">
       <c r="B13" s="6" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="14" spans="2:135">
       <c r="B14" s="6" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="15" spans="2:135">
       <c r="B15" s="6" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="16" spans="2:135">
       <c r="B16" s="6" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="17" spans="2:2">
       <c r="B17" s="6" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
   </sheetData>

</xml_diff>